<commit_message>
Updated for MAPD Preferred Plan
Updated for MAPD Preferred Plan
</commit_message>
<xml_diff>
--- a/cukesatdd/src/main/resources/database/PlanDocs/DCE_MBD_MAPD_Preferred_2022.xlsx
+++ b/cukesatdd/src/main/resources/database/PlanDocs/DCE_MBD_MAPD_Preferred_2022.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Git Hub Latest Project\mratdd\cukesatdd\src\main\resources\database\PlanDocs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E63B0466-F756-48A3-9F78-B3B04390F503}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{81943511-BC72-4247-B674-CF949D1B1D34}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" tabRatio="670" firstSheet="1" activeTab="4" xr2:uid="{1C4A239E-242B-48E7-9378-A03FDEBEBF97}"/>
   </bookViews>
@@ -42,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1374" uniqueCount="251">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1456" uniqueCount="257">
   <si>
     <t>Link Parameters</t>
   </si>
@@ -795,6 +795,24 @@
   </si>
   <si>
     <t>$0 for Tier 1, Tier 2, Tier 3 $345 for Tier 4, Tier 5</t>
+  </si>
+  <si>
+    <t>During the Coverage Gap Stage, you (or others on your behalf) will pay no more than 25% of the total cost for generic drugs or 25% of the total cost for brand name drugs, for any drug tier until the total amount you (or others on your behalf) and the drug manufacturer have paid reaches $7,050 in year-to-date out-of-pocket costs.</t>
+  </si>
+  <si>
+    <t>You enter the Catastrophic Coverage Stage after $7,050 is reached (excluding premiums), you will have to pay only one of the following through the end of the year: $3.95 copay for generic drugs, $9.85 copay for brand name drugs or a 15% coinsurance, whichever is greater. </t>
+  </si>
+  <si>
+    <t>Initial Coverage Stage Modal</t>
+  </si>
+  <si>
+    <t>In the Initial Coverage Stage, you (or others on your behalf) will pay a copay or coinsurance each time you fill a prescription, and the plan pays the rest. When your total drug costs—paid by you (or others on your behalf) and the plan—reach $4,430 you then move to the Coverage Gap Stage.</t>
+  </si>
+  <si>
+    <t>Deductible Coverage Stage Modal</t>
+  </si>
+  <si>
+    <t>In the Deductible Coverage Stage, you (or others on your behalf) will pay the full price for your prescription drugs until you reach the deductible amount. For some plans, this deductible will be $0 and you will enter the Initial Coverage Stage (below) with the first prescription you fill.</t>
   </si>
 </sst>
 </file>
@@ -805,7 +823,7 @@
     <numFmt numFmtId="6" formatCode="&quot;$&quot;#,##0_);[Red]\(&quot;$&quot;#,##0\)"/>
     <numFmt numFmtId="164" formatCode="&quot;$&quot;#,##0.00"/>
   </numFmts>
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -822,6 +840,13 @@
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF6A8759"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -847,7 +872,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -882,6 +907,13 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -5638,15 +5670,18 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D83056C1-4756-4383-A9FE-AD75C1A662C1}">
-  <dimension ref="A1:AL10"/>
+  <dimension ref="A1:AN10"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:XFD1"/>
+    <sheetView topLeftCell="AL1" workbookViewId="0">
+      <selection activeCell="AN1" sqref="AN1:AN10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="37" max="37" width="255.6328125" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:38" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:40" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -5761,8 +5796,14 @@
       <c r="AL1" s="4" t="s">
         <v>15</v>
       </c>
+      <c r="AM1" s="14" t="s">
+        <v>253</v>
+      </c>
+      <c r="AN1" s="14" t="s">
+        <v>255</v>
+      </c>
     </row>
-    <row r="2" spans="1:38" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:40" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>54</v>
       </c>
@@ -5871,14 +5912,20 @@
       <c r="AJ2" s="11">
         <v>0.28999999999999998</v>
       </c>
-      <c r="AK2" s="4" t="s">
-        <v>31</v>
-      </c>
-      <c r="AL2" s="4" t="s">
-        <v>32</v>
+      <c r="AK2" s="13" t="s">
+        <v>251</v>
+      </c>
+      <c r="AL2" s="13" t="s">
+        <v>252</v>
+      </c>
+      <c r="AM2" s="15" t="s">
+        <v>254</v>
+      </c>
+      <c r="AN2" s="15" t="s">
+        <v>256</v>
       </c>
     </row>
-    <row r="3" spans="1:38" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:40" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>60</v>
       </c>
@@ -5987,14 +6034,20 @@
       <c r="AJ3" s="11">
         <v>0.32</v>
       </c>
-      <c r="AK3" s="4" t="s">
-        <v>31</v>
-      </c>
-      <c r="AL3" s="4" t="s">
-        <v>32</v>
+      <c r="AK3" s="13" t="s">
+        <v>251</v>
+      </c>
+      <c r="AL3" s="13" t="s">
+        <v>252</v>
+      </c>
+      <c r="AM3" s="15" t="s">
+        <v>254</v>
+      </c>
+      <c r="AN3" s="15" t="s">
+        <v>256</v>
       </c>
     </row>
-    <row r="4" spans="1:38" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:40" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>74</v>
       </c>
@@ -6103,14 +6156,20 @@
       <c r="AJ4" s="11">
         <v>0.33</v>
       </c>
-      <c r="AK4" s="4" t="s">
-        <v>31</v>
-      </c>
-      <c r="AL4" s="4" t="s">
-        <v>32</v>
+      <c r="AK4" s="13" t="s">
+        <v>251</v>
+      </c>
+      <c r="AL4" s="13" t="s">
+        <v>252</v>
+      </c>
+      <c r="AM4" s="15" t="s">
+        <v>254</v>
+      </c>
+      <c r="AN4" s="15" t="s">
+        <v>256</v>
       </c>
     </row>
-    <row r="5" spans="1:38" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:40" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>87</v>
       </c>
@@ -6219,14 +6278,20 @@
       <c r="AJ5" s="11">
         <v>0.33</v>
       </c>
-      <c r="AK5" s="4" t="s">
-        <v>31</v>
-      </c>
-      <c r="AL5" s="4" t="s">
-        <v>32</v>
+      <c r="AK5" s="13" t="s">
+        <v>251</v>
+      </c>
+      <c r="AL5" s="13" t="s">
+        <v>252</v>
+      </c>
+      <c r="AM5" s="15" t="s">
+        <v>254</v>
+      </c>
+      <c r="AN5" s="15" t="s">
+        <v>256</v>
       </c>
     </row>
-    <row r="6" spans="1:38" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:40" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>117</v>
       </c>
@@ -6335,14 +6400,20 @@
       <c r="AJ6" s="11">
         <v>0.3</v>
       </c>
-      <c r="AK6" s="4" t="s">
-        <v>46</v>
-      </c>
-      <c r="AL6" s="4" t="s">
-        <v>32</v>
+      <c r="AK6" s="13" t="s">
+        <v>251</v>
+      </c>
+      <c r="AL6" s="13" t="s">
+        <v>252</v>
+      </c>
+      <c r="AM6" s="15" t="s">
+        <v>254</v>
+      </c>
+      <c r="AN6" s="15" t="s">
+        <v>256</v>
       </c>
     </row>
-    <row r="7" spans="1:38" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:40" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>120</v>
       </c>
@@ -6451,14 +6522,20 @@
       <c r="AJ7" s="11">
         <v>0.3</v>
       </c>
-      <c r="AK7" s="4" t="s">
-        <v>46</v>
-      </c>
-      <c r="AL7" s="4" t="s">
-        <v>32</v>
+      <c r="AK7" s="13" t="s">
+        <v>251</v>
+      </c>
+      <c r="AL7" s="13" t="s">
+        <v>252</v>
+      </c>
+      <c r="AM7" s="15" t="s">
+        <v>254</v>
+      </c>
+      <c r="AN7" s="15" t="s">
+        <v>256</v>
       </c>
     </row>
-    <row r="8" spans="1:38" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:40" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>122</v>
       </c>
@@ -6567,14 +6644,20 @@
       <c r="AJ8" s="11">
         <v>0.3</v>
       </c>
-      <c r="AK8" s="4" t="s">
-        <v>46</v>
-      </c>
-      <c r="AL8" s="4" t="s">
-        <v>32</v>
+      <c r="AK8" s="13" t="s">
+        <v>251</v>
+      </c>
+      <c r="AL8" s="13" t="s">
+        <v>252</v>
+      </c>
+      <c r="AM8" s="15" t="s">
+        <v>254</v>
+      </c>
+      <c r="AN8" s="15" t="s">
+        <v>256</v>
       </c>
     </row>
-    <row r="9" spans="1:38" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:40" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
         <v>124</v>
       </c>
@@ -6683,14 +6766,20 @@
       <c r="AJ9" s="11">
         <v>0.3</v>
       </c>
-      <c r="AK9" s="4" t="s">
-        <v>46</v>
-      </c>
-      <c r="AL9" s="4" t="s">
-        <v>32</v>
+      <c r="AK9" s="13" t="s">
+        <v>251</v>
+      </c>
+      <c r="AL9" s="13" t="s">
+        <v>252</v>
+      </c>
+      <c r="AM9" s="15" t="s">
+        <v>254</v>
+      </c>
+      <c r="AN9" s="15" t="s">
+        <v>256</v>
       </c>
     </row>
-    <row r="10" spans="1:38" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:40" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
         <v>126</v>
       </c>
@@ -6799,29 +6888,36 @@
       <c r="AJ10" s="11">
         <v>0.28000000000000003</v>
       </c>
-      <c r="AK10" s="4" t="s">
-        <v>31</v>
-      </c>
-      <c r="AL10" s="4" t="s">
-        <v>32</v>
+      <c r="AK10" s="13" t="s">
+        <v>251</v>
+      </c>
+      <c r="AL10" s="13" t="s">
+        <v>252</v>
+      </c>
+      <c r="AM10" s="15" t="s">
+        <v>254</v>
+      </c>
+      <c r="AN10" s="15" t="s">
+        <v>256</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4A27C4E5-FA49-4962-A0E2-1BF01BB105B2}">
-  <dimension ref="A1:AL11"/>
+  <dimension ref="A1:AN11"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C10" sqref="C10"/>
+    <sheetView topLeftCell="W1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="AN1" sqref="AN1:AN11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="1" spans="1:38" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:40" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -6936,8 +7032,14 @@
       <c r="AL1" s="4" t="s">
         <v>15</v>
       </c>
+      <c r="AM1" s="14" t="s">
+        <v>253</v>
+      </c>
+      <c r="AN1" s="14" t="s">
+        <v>255</v>
+      </c>
     </row>
-    <row r="2" spans="1:38" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:40" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>129</v>
       </c>
@@ -7046,14 +7148,20 @@
       <c r="AJ2" s="11">
         <v>0.27</v>
       </c>
-      <c r="AK2" s="4" t="s">
-        <v>31</v>
-      </c>
-      <c r="AL2" s="4" t="s">
-        <v>32</v>
+      <c r="AK2" s="13" t="s">
+        <v>251</v>
+      </c>
+      <c r="AL2" s="15" t="s">
+        <v>252</v>
+      </c>
+      <c r="AM2" s="15" t="s">
+        <v>254</v>
+      </c>
+      <c r="AN2" s="15" t="s">
+        <v>256</v>
       </c>
     </row>
-    <row r="3" spans="1:38" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:40" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>143</v>
       </c>
@@ -7162,14 +7270,20 @@
       <c r="AJ3" s="11">
         <v>0.3</v>
       </c>
-      <c r="AK3" s="4" t="s">
-        <v>31</v>
-      </c>
-      <c r="AL3" s="4" t="s">
-        <v>32</v>
+      <c r="AK3" s="13" t="s">
+        <v>251</v>
+      </c>
+      <c r="AL3" s="15" t="s">
+        <v>252</v>
+      </c>
+      <c r="AM3" s="15" t="s">
+        <v>254</v>
+      </c>
+      <c r="AN3" s="15" t="s">
+        <v>256</v>
       </c>
     </row>
-    <row r="4" spans="1:38" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:40" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>148</v>
       </c>
@@ -7278,14 +7392,20 @@
       <c r="AJ4" s="11">
         <v>0.33</v>
       </c>
-      <c r="AK4" s="4" t="s">
-        <v>31</v>
-      </c>
-      <c r="AL4" s="4" t="s">
-        <v>32</v>
+      <c r="AK4" s="13" t="s">
+        <v>251</v>
+      </c>
+      <c r="AL4" s="15" t="s">
+        <v>252</v>
+      </c>
+      <c r="AM4" s="15" t="s">
+        <v>254</v>
+      </c>
+      <c r="AN4" s="15" t="s">
+        <v>256</v>
       </c>
     </row>
-    <row r="5" spans="1:38" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:40" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>150</v>
       </c>
@@ -7394,14 +7514,20 @@
       <c r="AJ5" s="11">
         <v>0.3</v>
       </c>
-      <c r="AK5" s="4" t="s">
-        <v>31</v>
-      </c>
-      <c r="AL5" s="4" t="s">
-        <v>32</v>
+      <c r="AK5" s="13" t="s">
+        <v>251</v>
+      </c>
+      <c r="AL5" s="15" t="s">
+        <v>252</v>
+      </c>
+      <c r="AM5" s="15" t="s">
+        <v>254</v>
+      </c>
+      <c r="AN5" s="15" t="s">
+        <v>256</v>
       </c>
     </row>
-    <row r="6" spans="1:38" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:40" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>153</v>
       </c>
@@ -7510,14 +7636,20 @@
       <c r="AJ6" s="11">
         <v>0.28999999999999998</v>
       </c>
-      <c r="AK6" s="4" t="s">
-        <v>31</v>
-      </c>
-      <c r="AL6" s="4" t="s">
-        <v>32</v>
+      <c r="AK6" s="13" t="s">
+        <v>251</v>
+      </c>
+      <c r="AL6" s="15" t="s">
+        <v>252</v>
+      </c>
+      <c r="AM6" s="15" t="s">
+        <v>254</v>
+      </c>
+      <c r="AN6" s="15" t="s">
+        <v>256</v>
       </c>
     </row>
-    <row r="7" spans="1:38" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:40" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>155</v>
       </c>
@@ -7626,14 +7758,20 @@
       <c r="AJ7" s="11">
         <v>0.33</v>
       </c>
-      <c r="AK7" s="4" t="s">
-        <v>31</v>
-      </c>
-      <c r="AL7" s="4" t="s">
-        <v>32</v>
+      <c r="AK7" s="13" t="s">
+        <v>251</v>
+      </c>
+      <c r="AL7" s="15" t="s">
+        <v>252</v>
+      </c>
+      <c r="AM7" s="15" t="s">
+        <v>254</v>
+      </c>
+      <c r="AN7" s="15" t="s">
+        <v>256</v>
       </c>
     </row>
-    <row r="8" spans="1:38" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:40" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>157</v>
       </c>
@@ -7742,14 +7880,20 @@
       <c r="AJ8" s="11">
         <v>0.28000000000000003</v>
       </c>
-      <c r="AK8" s="4" t="s">
-        <v>31</v>
-      </c>
-      <c r="AL8" s="4" t="s">
-        <v>32</v>
+      <c r="AK8" s="13" t="s">
+        <v>251</v>
+      </c>
+      <c r="AL8" s="15" t="s">
+        <v>252</v>
+      </c>
+      <c r="AM8" s="15" t="s">
+        <v>254</v>
+      </c>
+      <c r="AN8" s="15" t="s">
+        <v>256</v>
       </c>
     </row>
-    <row r="9" spans="1:38" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:40" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
         <v>159</v>
       </c>
@@ -7858,14 +8002,20 @@
       <c r="AJ9" s="11">
         <v>0.33</v>
       </c>
-      <c r="AK9" s="4" t="s">
-        <v>31</v>
-      </c>
-      <c r="AL9" s="4" t="s">
-        <v>32</v>
+      <c r="AK9" s="13" t="s">
+        <v>251</v>
+      </c>
+      <c r="AL9" s="15" t="s">
+        <v>252</v>
+      </c>
+      <c r="AM9" s="15" t="s">
+        <v>254</v>
+      </c>
+      <c r="AN9" s="15" t="s">
+        <v>256</v>
       </c>
     </row>
-    <row r="10" spans="1:38" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:40" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
         <v>161</v>
       </c>
@@ -7974,14 +8124,20 @@
       <c r="AJ10" s="11">
         <v>0.33</v>
       </c>
-      <c r="AK10" s="4" t="s">
-        <v>31</v>
-      </c>
-      <c r="AL10" s="4" t="s">
-        <v>32</v>
+      <c r="AK10" s="13" t="s">
+        <v>251</v>
+      </c>
+      <c r="AL10" s="15" t="s">
+        <v>252</v>
+      </c>
+      <c r="AM10" s="15" t="s">
+        <v>254</v>
+      </c>
+      <c r="AN10" s="15" t="s">
+        <v>256</v>
       </c>
     </row>
-    <row r="11" spans="1:38" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:40" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
         <v>164</v>
       </c>
@@ -8090,11 +8246,17 @@
       <c r="AJ11" s="11">
         <v>0.33</v>
       </c>
-      <c r="AK11" s="4" t="s">
-        <v>31</v>
-      </c>
-      <c r="AL11" s="4" t="s">
-        <v>32</v>
+      <c r="AK11" s="13" t="s">
+        <v>251</v>
+      </c>
+      <c r="AL11" s="15" t="s">
+        <v>252</v>
+      </c>
+      <c r="AM11" s="15" t="s">
+        <v>254</v>
+      </c>
+      <c r="AN11" s="15" t="s">
+        <v>256</v>
       </c>
     </row>
   </sheetData>
@@ -8105,15 +8267,15 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AA9DB233-EC17-4F84-BE92-BC90609DA00E}">
-  <dimension ref="A1:AL11"/>
+  <dimension ref="A1:AN11"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D9" sqref="D9"/>
+    <sheetView topLeftCell="V1" workbookViewId="0">
+      <selection activeCell="AN1" sqref="AN1:AN9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="1" spans="1:38" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:40" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -8228,8 +8390,14 @@
       <c r="AL1" s="4" t="s">
         <v>15</v>
       </c>
+      <c r="AM1" s="14" t="s">
+        <v>253</v>
+      </c>
+      <c r="AN1" s="14" t="s">
+        <v>255</v>
+      </c>
     </row>
-    <row r="2" spans="1:38" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:40" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>166</v>
       </c>
@@ -8338,14 +8506,20 @@
       <c r="AJ2" s="11">
         <v>0.31</v>
       </c>
-      <c r="AK2" s="4" t="s">
-        <v>31</v>
-      </c>
-      <c r="AL2" s="4" t="s">
-        <v>32</v>
+      <c r="AK2" s="13" t="s">
+        <v>251</v>
+      </c>
+      <c r="AL2" s="15" t="s">
+        <v>252</v>
+      </c>
+      <c r="AM2" s="15" t="s">
+        <v>254</v>
+      </c>
+      <c r="AN2" s="15" t="s">
+        <v>256</v>
       </c>
     </row>
-    <row r="3" spans="1:38" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:40" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>171</v>
       </c>
@@ -8454,14 +8628,20 @@
       <c r="AJ3" s="11">
         <v>0.33</v>
       </c>
-      <c r="AK3" s="4" t="s">
-        <v>31</v>
-      </c>
-      <c r="AL3" s="4" t="s">
-        <v>32</v>
+      <c r="AK3" s="13" t="s">
+        <v>251</v>
+      </c>
+      <c r="AL3" s="15" t="s">
+        <v>252</v>
+      </c>
+      <c r="AM3" s="15" t="s">
+        <v>254</v>
+      </c>
+      <c r="AN3" s="15" t="s">
+        <v>256</v>
       </c>
     </row>
-    <row r="4" spans="1:38" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:40" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>173</v>
       </c>
@@ -8570,14 +8750,20 @@
       <c r="AJ4" s="11">
         <v>0.33</v>
       </c>
-      <c r="AK4" s="4" t="s">
-        <v>31</v>
-      </c>
-      <c r="AL4" s="4" t="s">
-        <v>32</v>
+      <c r="AK4" s="13" t="s">
+        <v>251</v>
+      </c>
+      <c r="AL4" s="15" t="s">
+        <v>252</v>
+      </c>
+      <c r="AM4" s="15" t="s">
+        <v>254</v>
+      </c>
+      <c r="AN4" s="15" t="s">
+        <v>256</v>
       </c>
     </row>
-    <row r="5" spans="1:38" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:40" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>177</v>
       </c>
@@ -8686,14 +8872,20 @@
       <c r="AJ5" s="11">
         <v>0.28999999999999998</v>
       </c>
-      <c r="AK5" s="4" t="s">
-        <v>31</v>
-      </c>
-      <c r="AL5" s="4" t="s">
-        <v>32</v>
+      <c r="AK5" s="13" t="s">
+        <v>251</v>
+      </c>
+      <c r="AL5" s="15" t="s">
+        <v>252</v>
+      </c>
+      <c r="AM5" s="15" t="s">
+        <v>254</v>
+      </c>
+      <c r="AN5" s="15" t="s">
+        <v>256</v>
       </c>
     </row>
-    <row r="6" spans="1:38" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:40" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>184</v>
       </c>
@@ -8802,14 +8994,20 @@
       <c r="AJ6" s="11">
         <v>0.33</v>
       </c>
-      <c r="AK6" s="4" t="s">
-        <v>31</v>
-      </c>
-      <c r="AL6" s="4" t="s">
-        <v>32</v>
+      <c r="AK6" s="13" t="s">
+        <v>251</v>
+      </c>
+      <c r="AL6" s="15" t="s">
+        <v>252</v>
+      </c>
+      <c r="AM6" s="15" t="s">
+        <v>254</v>
+      </c>
+      <c r="AN6" s="15" t="s">
+        <v>256</v>
       </c>
     </row>
-    <row r="7" spans="1:38" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:40" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>186</v>
       </c>
@@ -8918,14 +9116,20 @@
       <c r="AJ7" s="11">
         <v>0.28999999999999998</v>
       </c>
-      <c r="AK7" s="4" t="s">
-        <v>31</v>
-      </c>
-      <c r="AL7" s="4" t="s">
-        <v>32</v>
+      <c r="AK7" s="13" t="s">
+        <v>251</v>
+      </c>
+      <c r="AL7" s="15" t="s">
+        <v>252</v>
+      </c>
+      <c r="AM7" s="15" t="s">
+        <v>254</v>
+      </c>
+      <c r="AN7" s="15" t="s">
+        <v>256</v>
       </c>
     </row>
-    <row r="8" spans="1:38" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:40" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>188</v>
       </c>
@@ -9034,14 +9238,20 @@
       <c r="AJ8" s="11">
         <v>0.33</v>
       </c>
-      <c r="AK8" s="4" t="s">
-        <v>31</v>
-      </c>
-      <c r="AL8" s="4" t="s">
-        <v>32</v>
+      <c r="AK8" s="13" t="s">
+        <v>251</v>
+      </c>
+      <c r="AL8" s="15" t="s">
+        <v>252</v>
+      </c>
+      <c r="AM8" s="15" t="s">
+        <v>254</v>
+      </c>
+      <c r="AN8" s="15" t="s">
+        <v>256</v>
       </c>
     </row>
-    <row r="9" spans="1:38" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:40" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
         <v>190</v>
       </c>
@@ -9150,14 +9360,20 @@
       <c r="AJ9" s="11">
         <v>0.28999999999999998</v>
       </c>
-      <c r="AK9" s="4" t="s">
-        <v>31</v>
-      </c>
-      <c r="AL9" s="4" t="s">
-        <v>32</v>
+      <c r="AK9" s="13" t="s">
+        <v>251</v>
+      </c>
+      <c r="AL9" s="15" t="s">
+        <v>252</v>
+      </c>
+      <c r="AM9" s="15" t="s">
+        <v>254</v>
+      </c>
+      <c r="AN9" s="15" t="s">
+        <v>256</v>
       </c>
     </row>
-    <row r="10" spans="1:38" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:40" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
         <v>192</v>
       </c>
@@ -9266,14 +9482,20 @@
       <c r="AJ10" s="11">
         <v>0.31</v>
       </c>
-      <c r="AK10" s="4" t="s">
-        <v>31</v>
-      </c>
-      <c r="AL10" s="4" t="s">
-        <v>32</v>
+      <c r="AK10" s="13" t="s">
+        <v>251</v>
+      </c>
+      <c r="AL10" s="15" t="s">
+        <v>252</v>
+      </c>
+      <c r="AM10" s="15" t="s">
+        <v>254</v>
+      </c>
+      <c r="AN10" s="15" t="s">
+        <v>256</v>
       </c>
     </row>
-    <row r="11" spans="1:38" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:40" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
         <v>197</v>
       </c>
@@ -9382,11 +9604,17 @@
       <c r="AJ11" s="11">
         <v>0.33</v>
       </c>
-      <c r="AK11" s="4" t="s">
-        <v>31</v>
-      </c>
-      <c r="AL11" s="4" t="s">
-        <v>32</v>
+      <c r="AK11" s="13" t="s">
+        <v>251</v>
+      </c>
+      <c r="AL11" s="15" t="s">
+        <v>252</v>
+      </c>
+      <c r="AM11" s="15" t="s">
+        <v>254</v>
+      </c>
+      <c r="AN11" s="15" t="s">
+        <v>256</v>
       </c>
     </row>
   </sheetData>
@@ -9396,15 +9624,15 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BFA1B4B9-D9BF-444A-891C-8F4857F671C7}">
-  <dimension ref="A1:AL9"/>
+  <dimension ref="A1:AN11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A8" sqref="A8"/>
+      <selection activeCell="F10" sqref="F10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="1" spans="1:38" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:40" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -9519,8 +9747,14 @@
       <c r="AL1" s="4" t="s">
         <v>15</v>
       </c>
+      <c r="AM1" s="14" t="s">
+        <v>253</v>
+      </c>
+      <c r="AN1" s="14" t="s">
+        <v>255</v>
+      </c>
     </row>
-    <row r="2" spans="1:38" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:40" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>200</v>
       </c>
@@ -9629,14 +9863,20 @@
       <c r="AJ2" s="11">
         <v>0.28999999999999998</v>
       </c>
-      <c r="AK2" s="4" t="s">
-        <v>31</v>
-      </c>
-      <c r="AL2" s="4" t="s">
-        <v>32</v>
+      <c r="AK2" s="13" t="s">
+        <v>251</v>
+      </c>
+      <c r="AL2" s="15" t="s">
+        <v>252</v>
+      </c>
+      <c r="AM2" s="15" t="s">
+        <v>254</v>
+      </c>
+      <c r="AN2" s="15" t="s">
+        <v>256</v>
       </c>
     </row>
-    <row r="3" spans="1:38" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:40" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>205</v>
       </c>
@@ -9745,14 +9985,20 @@
       <c r="AJ3" s="11">
         <v>0.25</v>
       </c>
-      <c r="AK3" s="4" t="s">
-        <v>31</v>
-      </c>
-      <c r="AL3" s="4" t="s">
-        <v>32</v>
+      <c r="AK3" s="13" t="s">
+        <v>251</v>
+      </c>
+      <c r="AL3" s="15" t="s">
+        <v>252</v>
+      </c>
+      <c r="AM3" s="15" t="s">
+        <v>254</v>
+      </c>
+      <c r="AN3" s="15" t="s">
+        <v>256</v>
       </c>
     </row>
-    <row r="4" spans="1:38" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:40" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>208</v>
       </c>
@@ -9861,14 +10107,20 @@
       <c r="AJ4" s="11">
         <v>0.25</v>
       </c>
-      <c r="AK4" s="4" t="s">
-        <v>31</v>
-      </c>
-      <c r="AL4" s="4" t="s">
-        <v>32</v>
+      <c r="AK4" s="13" t="s">
+        <v>251</v>
+      </c>
+      <c r="AL4" s="15" t="s">
+        <v>252</v>
+      </c>
+      <c r="AM4" s="15" t="s">
+        <v>254</v>
+      </c>
+      <c r="AN4" s="15" t="s">
+        <v>256</v>
       </c>
     </row>
-    <row r="5" spans="1:38" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:40" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>212</v>
       </c>
@@ -9977,14 +10229,20 @@
       <c r="AJ5" s="11">
         <v>0.28999999999999998</v>
       </c>
-      <c r="AK5" s="4" t="s">
-        <v>31</v>
-      </c>
-      <c r="AL5" s="4" t="s">
-        <v>32</v>
+      <c r="AK5" s="13" t="s">
+        <v>251</v>
+      </c>
+      <c r="AL5" s="15" t="s">
+        <v>252</v>
+      </c>
+      <c r="AM5" s="15" t="s">
+        <v>254</v>
+      </c>
+      <c r="AN5" s="15" t="s">
+        <v>256</v>
       </c>
     </row>
-    <row r="6" spans="1:38" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:40" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>214</v>
       </c>
@@ -10093,14 +10351,20 @@
       <c r="AJ6" s="11">
         <v>0.28000000000000003</v>
       </c>
-      <c r="AK6" s="4" t="s">
-        <v>31</v>
-      </c>
-      <c r="AL6" s="4" t="s">
-        <v>32</v>
+      <c r="AK6" s="13" t="s">
+        <v>251</v>
+      </c>
+      <c r="AL6" s="15" t="s">
+        <v>252</v>
+      </c>
+      <c r="AM6" s="15" t="s">
+        <v>254</v>
+      </c>
+      <c r="AN6" s="15" t="s">
+        <v>256</v>
       </c>
     </row>
-    <row r="7" spans="1:38" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:40" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>216</v>
       </c>
@@ -10209,14 +10473,20 @@
       <c r="AJ7" s="11">
         <v>0.28000000000000003</v>
       </c>
-      <c r="AK7" s="4" t="s">
-        <v>31</v>
-      </c>
-      <c r="AL7" s="4" t="s">
-        <v>32</v>
+      <c r="AK7" s="13" t="s">
+        <v>251</v>
+      </c>
+      <c r="AL7" s="15" t="s">
+        <v>252</v>
+      </c>
+      <c r="AM7" s="15" t="s">
+        <v>254</v>
+      </c>
+      <c r="AN7" s="15" t="s">
+        <v>256</v>
       </c>
     </row>
-    <row r="8" spans="1:38" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:40" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>218</v>
       </c>
@@ -10325,14 +10595,20 @@
       <c r="AJ8" s="11">
         <v>0.28999999999999998</v>
       </c>
-      <c r="AK8" s="4" t="s">
-        <v>31</v>
-      </c>
-      <c r="AL8" s="4" t="s">
-        <v>32</v>
+      <c r="AK8" s="13" t="s">
+        <v>251</v>
+      </c>
+      <c r="AL8" s="15" t="s">
+        <v>252</v>
+      </c>
+      <c r="AM8" s="15" t="s">
+        <v>254</v>
+      </c>
+      <c r="AN8" s="15" t="s">
+        <v>256</v>
       </c>
     </row>
-    <row r="9" spans="1:38" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:40" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
         <v>220</v>
       </c>
@@ -10441,12 +10717,28 @@
       <c r="AJ9" s="11">
         <v>0.28000000000000003</v>
       </c>
-      <c r="AK9" s="4" t="s">
-        <v>31</v>
-      </c>
-      <c r="AL9" s="4" t="s">
-        <v>32</v>
-      </c>
+      <c r="AK9" s="13" t="s">
+        <v>251</v>
+      </c>
+      <c r="AL9" s="15" t="s">
+        <v>252</v>
+      </c>
+      <c r="AM9" s="15" t="s">
+        <v>254</v>
+      </c>
+      <c r="AN9" s="15" t="s">
+        <v>256</v>
+      </c>
+    </row>
+    <row r="10" spans="1:40" x14ac:dyDescent="0.35">
+      <c r="AK10" s="13"/>
+      <c r="AL10" s="13"/>
+      <c r="AM10" s="15"/>
+    </row>
+    <row r="11" spans="1:40" x14ac:dyDescent="0.35">
+      <c r="AK11" s="13"/>
+      <c r="AL11" s="13"/>
+      <c r="AM11" s="15"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>